<commit_message>
kth smallest in Array
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t xml:space="preserve">Questions by Love Babbar:</t>
   </si>
@@ -37,25 +37,25 @@
     <t xml:space="preserve">Done [yes or no] </t>
   </si>
   <si>
+    <t xml:space="preserve">Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse the array</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;yes&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reverse the array</t>
-  </si>
-  <si>
     <t xml:space="preserve">Find the maximum and minimum element in an array</t>
   </si>
   <si>
+    <t xml:space="preserve">Find the "Kth" max and min element of an array </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given an array which consists of only 0, 1 and 2. Sort the array without using any sorting algo</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;-&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Find the "Kth" max and min element of an array </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Given an array which consists of only 0, 1 and 2. Sort the array without using any sorting algo</t>
   </si>
   <si>
     <t xml:space="preserve">Move all the negative elements to one side of the array </t>
@@ -1666,10 +1666,10 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.93"/>
@@ -1698,417 +1698,415 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="8"/>
       <c r="C42" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6"/>
       <c r="B43" s="8"/>
       <c r="C43" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,7 +2117,7 @@
         <v>45</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2128,7 @@
         <v>46</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,7 +2139,7 @@
         <v>47</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2150,7 @@
         <v>48</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,7 +2161,7 @@
         <v>49</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2174,7 +2172,7 @@
         <v>50</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2185,7 +2183,7 @@
         <v>51</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2194,7 @@
         <v>52</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2207,7 +2205,7 @@
         <v>53</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,7 +2216,7 @@
         <v>54</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,7 +2232,7 @@
         <v>56</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,7 +2243,7 @@
         <v>57</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,7 +2254,7 @@
         <v>58</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,7 +2265,7 @@
         <v>59</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2278,7 +2276,7 @@
         <v>60</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,7 +2287,7 @@
         <v>61</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2300,7 +2298,7 @@
         <v>62</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2309,7 @@
         <v>63</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2320,7 @@
         <v>64</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2333,7 +2331,7 @@
         <v>65</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,7 +2342,7 @@
         <v>66</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,7 +2353,7 @@
         <v>67</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,7 +2364,7 @@
         <v>68</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,7 +2375,7 @@
         <v>69</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,7 +2386,7 @@
         <v>70</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,7 +2397,7 @@
         <v>71</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2410,7 +2408,7 @@
         <v>72</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2419,7 @@
         <v>73</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,7 +2430,7 @@
         <v>74</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,7 +2441,7 @@
         <v>75</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2454,7 +2452,7 @@
         <v>76</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +2463,7 @@
         <v>77</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2474,7 @@
         <v>78</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,7 +2485,7 @@
         <v>79</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,7 +2496,7 @@
         <v>80</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2507,7 @@
         <v>81</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2520,7 +2518,7 @@
         <v>82</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,7 +2529,7 @@
         <v>83</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2542,7 +2540,7 @@
         <v>84</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2553,7 +2551,7 @@
         <v>85</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2564,7 +2562,7 @@
         <v>86</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2575,7 +2573,7 @@
         <v>87</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,7 +2584,7 @@
         <v>88</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2597,7 +2595,7 @@
         <v>89</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2608,7 +2606,7 @@
         <v>90</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,7 +2617,7 @@
         <v>91</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2628,7 @@
         <v>92</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2641,7 +2639,7 @@
         <v>93</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,7 +2650,7 @@
         <v>94</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,7 +2661,7 @@
         <v>95</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,7 +2672,7 @@
         <v>96</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2685,7 +2683,7 @@
         <v>97</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,7 +2694,7 @@
         <v>98</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2712,7 +2710,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,7 +2721,7 @@
         <v>101</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2734,7 +2732,7 @@
         <v>102</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2743,7 @@
         <v>103</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,7 +2754,7 @@
         <v>104</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2767,7 +2765,7 @@
         <v>105</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,7 +2776,7 @@
         <v>106</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2789,7 +2787,7 @@
         <v>107</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,7 +2798,7 @@
         <v>108</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,7 +2809,7 @@
         <v>109</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2822,7 +2820,7 @@
         <v>110</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,7 +2831,7 @@
         <v>111</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2844,7 +2842,7 @@
         <v>112</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +2853,7 @@
         <v>113</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2866,7 +2864,7 @@
         <v>114</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2877,7 +2875,7 @@
         <v>115</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2888,7 +2886,7 @@
         <v>116</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2899,7 +2897,7 @@
         <v>117</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2910,7 +2908,7 @@
         <v>118</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2921,7 +2919,7 @@
         <v>119</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2932,7 +2930,7 @@
         <v>120</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,7 +2941,7 @@
         <v>121</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2954,7 +2952,7 @@
         <v>122</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +2963,7 @@
         <v>123</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2976,7 +2974,7 @@
         <v>124</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2987,7 +2985,7 @@
         <v>125</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2998,7 +2996,7 @@
         <v>126</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,7 +3007,7 @@
         <v>127</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,7 +3018,7 @@
         <v>128</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3031,7 +3029,7 @@
         <v>129</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3042,7 +3040,7 @@
         <v>130</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3053,7 +3051,7 @@
         <v>131</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3064,7 +3062,7 @@
         <v>132</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,7 +3073,7 @@
         <v>133</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3086,7 +3084,7 @@
         <v>134</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,7 +3095,7 @@
         <v>135</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3112,7 +3110,7 @@
         <v>137</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,7 +3121,7 @@
         <v>138</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,7 +3132,7 @@
         <v>139</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3145,7 +3143,7 @@
         <v>140</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3156,7 +3154,7 @@
         <v>141</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3167,7 +3165,7 @@
         <v>142</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3178,7 +3176,7 @@
         <v>143</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3189,7 +3187,7 @@
         <v>144</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3200,7 +3198,7 @@
         <v>145</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,7 +3209,7 @@
         <v>146</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3222,7 +3220,7 @@
         <v>147</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3233,7 +3231,7 @@
         <v>148</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,7 +3242,7 @@
         <v>149</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,7 +3253,7 @@
         <v>150</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3266,7 +3264,7 @@
         <v>151</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3277,7 +3275,7 @@
         <v>152</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,7 +3286,7 @@
         <v>153</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3299,7 +3297,7 @@
         <v>154</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3310,7 +3308,7 @@
         <v>155</v>
       </c>
       <c r="C157" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3321,7 +3319,7 @@
         <v>156</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3332,7 +3330,7 @@
         <v>157</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3343,7 +3341,7 @@
         <v>158</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3354,7 +3352,7 @@
         <v>159</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3365,7 +3363,7 @@
         <v>160</v>
       </c>
       <c r="C162" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3376,7 +3374,7 @@
         <v>161</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3385,7 @@
         <v>162</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3398,7 +3396,7 @@
         <v>163</v>
       </c>
       <c r="C165" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3409,7 +3407,7 @@
         <v>164</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,7 +3418,7 @@
         <v>165</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3431,7 +3429,7 @@
         <v>166</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,7 +3440,7 @@
         <v>167</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3453,7 +3451,7 @@
         <v>168</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3464,7 +3462,7 @@
         <v>169</v>
       </c>
       <c r="C171" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3475,7 +3473,7 @@
         <v>170</v>
       </c>
       <c r="C172" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3486,7 +3484,7 @@
         <v>171</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3497,7 +3495,7 @@
         <v>172</v>
       </c>
       <c r="C174" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3512,7 +3510,7 @@
         <v>174</v>
       </c>
       <c r="C177" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3523,7 +3521,7 @@
         <v>175</v>
       </c>
       <c r="C178" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3534,7 +3532,7 @@
         <v>176</v>
       </c>
       <c r="C179" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3545,7 +3543,7 @@
         <v>177</v>
       </c>
       <c r="C180" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3556,7 +3554,7 @@
         <v>178</v>
       </c>
       <c r="C181" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3567,7 +3565,7 @@
         <v>179</v>
       </c>
       <c r="C182" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,7 +3576,7 @@
         <v>180</v>
       </c>
       <c r="C183" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,7 +3587,7 @@
         <v>181</v>
       </c>
       <c r="C184" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3600,7 +3598,7 @@
         <v>182</v>
       </c>
       <c r="C185" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3611,7 +3609,7 @@
         <v>183</v>
       </c>
       <c r="C186" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3622,7 +3620,7 @@
         <v>184</v>
       </c>
       <c r="C187" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,7 +3631,7 @@
         <v>185</v>
       </c>
       <c r="C188" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3644,7 +3642,7 @@
         <v>186</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3655,7 +3653,7 @@
         <v>187</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,7 +3664,7 @@
         <v>188</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3677,7 +3675,7 @@
         <v>189</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,7 +3686,7 @@
         <v>190</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3699,7 +3697,7 @@
         <v>191</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3710,7 +3708,7 @@
         <v>192</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3721,7 +3719,7 @@
         <v>193</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3732,7 +3730,7 @@
         <v>194</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,7 +3741,7 @@
         <v>195</v>
       </c>
       <c r="C198" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,7 +3752,7 @@
         <v>196</v>
       </c>
       <c r="C199" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3765,7 +3763,7 @@
         <v>197</v>
       </c>
       <c r="C200" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3776,7 +3774,7 @@
         <v>198</v>
       </c>
       <c r="C201" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3787,7 +3785,7 @@
         <v>199</v>
       </c>
       <c r="C202" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3798,7 +3796,7 @@
         <v>200</v>
       </c>
       <c r="C203" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3809,7 +3807,7 @@
         <v>201</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,7 +3818,7 @@
         <v>202</v>
       </c>
       <c r="C205" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,7 +3829,7 @@
         <v>203</v>
       </c>
       <c r="C206" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3842,7 +3840,7 @@
         <v>204</v>
       </c>
       <c r="C207" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3853,7 +3851,7 @@
         <v>205</v>
       </c>
       <c r="C208" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3864,7 +3862,7 @@
         <v>206</v>
       </c>
       <c r="C209" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,7 +3873,7 @@
         <v>207</v>
       </c>
       <c r="C210" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3886,7 +3884,7 @@
         <v>208</v>
       </c>
       <c r="C211" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3907,7 +3905,7 @@
         <v>210</v>
       </c>
       <c r="C214" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3918,7 +3916,7 @@
         <v>211</v>
       </c>
       <c r="C215" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3929,7 +3927,7 @@
         <v>212</v>
       </c>
       <c r="C216" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3940,7 +3938,7 @@
         <v>213</v>
       </c>
       <c r="C217" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3951,7 +3949,7 @@
         <v>214</v>
       </c>
       <c r="C218" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3962,7 +3960,7 @@
         <v>215</v>
       </c>
       <c r="C219" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3973,7 +3971,7 @@
         <v>216</v>
       </c>
       <c r="C220" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3984,7 +3982,7 @@
         <v>217</v>
       </c>
       <c r="C221" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,7 +3993,7 @@
         <v>218</v>
       </c>
       <c r="C222" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4006,7 +4004,7 @@
         <v>219</v>
       </c>
       <c r="C223" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4017,7 +4015,7 @@
         <v>220</v>
       </c>
       <c r="C224" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4028,7 +4026,7 @@
         <v>221</v>
       </c>
       <c r="C225" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4039,7 +4037,7 @@
         <v>222</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4050,7 +4048,7 @@
         <v>223</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4061,7 +4059,7 @@
         <v>224</v>
       </c>
       <c r="C228" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4072,7 +4070,7 @@
         <v>225</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4083,7 +4081,7 @@
         <v>226</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4094,7 +4092,7 @@
         <v>227</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4105,7 +4103,7 @@
         <v>228</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4116,7 +4114,7 @@
         <v>229</v>
       </c>
       <c r="C233" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4127,7 +4125,7 @@
         <v>230</v>
       </c>
       <c r="C234" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4138,7 +4136,7 @@
         <v>231</v>
       </c>
       <c r="C235" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,7 +4155,7 @@
         <v>233</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4168,7 +4166,7 @@
         <v>234</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4179,7 +4177,7 @@
         <v>235</v>
       </c>
       <c r="C240" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4190,7 +4188,7 @@
         <v>236</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4201,7 +4199,7 @@
         <v>237</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,7 +4210,7 @@
         <v>238</v>
       </c>
       <c r="C243" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4223,7 +4221,7 @@
         <v>239</v>
       </c>
       <c r="C244" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4234,7 +4232,7 @@
         <v>240</v>
       </c>
       <c r="C245" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4245,7 +4243,7 @@
         <v>241</v>
       </c>
       <c r="C246" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4256,7 +4254,7 @@
         <v>242</v>
       </c>
       <c r="C247" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4267,7 +4265,7 @@
         <v>243</v>
       </c>
       <c r="C248" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4278,7 +4276,7 @@
         <v>244</v>
       </c>
       <c r="C249" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4289,7 +4287,7 @@
         <v>245</v>
       </c>
       <c r="C250" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4300,7 +4298,7 @@
         <v>246</v>
       </c>
       <c r="C251" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4311,7 +4309,7 @@
         <v>247</v>
       </c>
       <c r="C252" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4322,7 +4320,7 @@
         <v>248</v>
       </c>
       <c r="C253" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4333,7 +4331,7 @@
         <v>249</v>
       </c>
       <c r="C254" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4344,7 +4342,7 @@
         <v>250</v>
       </c>
       <c r="C255" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4355,7 +4353,7 @@
         <v>251</v>
       </c>
       <c r="C256" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4366,7 +4364,7 @@
         <v>252</v>
       </c>
       <c r="C257" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4377,7 +4375,7 @@
         <v>253</v>
       </c>
       <c r="C258" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4388,7 +4386,7 @@
         <v>254</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4399,7 +4397,7 @@
         <v>255</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,7 +4408,7 @@
         <v>256</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4421,7 +4419,7 @@
         <v>257</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4432,7 +4430,7 @@
         <v>258</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4443,7 +4441,7 @@
         <v>259</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4454,7 +4452,7 @@
         <v>260</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4465,7 +4463,7 @@
         <v>261</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4476,7 +4474,7 @@
         <v>262</v>
       </c>
       <c r="C267" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4487,7 +4485,7 @@
         <v>263</v>
       </c>
       <c r="C268" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4498,7 +4496,7 @@
         <v>264</v>
       </c>
       <c r="C269" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4509,7 +4507,7 @@
         <v>265</v>
       </c>
       <c r="C270" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4520,7 +4518,7 @@
         <v>89</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4531,7 +4529,7 @@
         <v>266</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4550,7 +4548,7 @@
         <v>268</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4561,7 +4559,7 @@
         <v>269</v>
       </c>
       <c r="C276" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4572,7 +4570,7 @@
         <v>270</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4583,7 +4581,7 @@
         <v>271</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4594,7 +4592,7 @@
         <v>272</v>
       </c>
       <c r="C279" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4605,7 +4603,7 @@
         <v>273</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4616,7 +4614,7 @@
         <v>274</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4627,7 +4625,7 @@
         <v>275</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4638,7 +4636,7 @@
         <v>276</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4649,7 +4647,7 @@
         <v>277</v>
       </c>
       <c r="C284" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4660,7 +4658,7 @@
         <v>278</v>
       </c>
       <c r="C285" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4671,7 +4669,7 @@
         <v>279</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,7 +4680,7 @@
         <v>280</v>
       </c>
       <c r="C287" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4693,7 +4691,7 @@
         <v>281</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4704,7 +4702,7 @@
         <v>282</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4715,7 +4713,7 @@
         <v>283</v>
       </c>
       <c r="C290" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4726,7 +4724,7 @@
         <v>284</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4737,7 +4735,7 @@
         <v>285</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4748,7 +4746,7 @@
         <v>286</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4767,7 +4765,7 @@
         <v>288</v>
       </c>
       <c r="C296" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4778,7 +4776,7 @@
         <v>289</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4789,7 +4787,7 @@
         <v>290</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4800,7 +4798,7 @@
         <v>291</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4811,7 +4809,7 @@
         <v>292</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4822,7 +4820,7 @@
         <v>293</v>
       </c>
       <c r="C301" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4833,7 +4831,7 @@
         <v>294</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4844,7 +4842,7 @@
         <v>295</v>
       </c>
       <c r="C303" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4855,7 +4853,7 @@
         <v>296</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4866,7 +4864,7 @@
         <v>297</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4877,7 +4875,7 @@
         <v>298</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4888,7 +4886,7 @@
         <v>299</v>
       </c>
       <c r="C307" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4899,7 +4897,7 @@
         <v>300</v>
       </c>
       <c r="C308" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4910,7 +4908,7 @@
         <v>301</v>
       </c>
       <c r="C309" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4921,7 +4919,7 @@
         <v>302</v>
       </c>
       <c r="C310" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4932,7 +4930,7 @@
         <v>303</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4943,7 +4941,7 @@
         <v>304</v>
       </c>
       <c r="C312" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,7 +4952,7 @@
         <v>305</v>
       </c>
       <c r="C313" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4965,7 +4963,7 @@
         <v>306</v>
       </c>
       <c r="C314" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4976,7 +4974,7 @@
         <v>307</v>
       </c>
       <c r="C315" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4987,7 +4985,7 @@
         <v>308</v>
       </c>
       <c r="C316" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4998,7 +4996,7 @@
         <v>309</v>
       </c>
       <c r="C317" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5009,7 +5007,7 @@
         <v>310</v>
       </c>
       <c r="C318" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5020,7 +5018,7 @@
         <v>311</v>
       </c>
       <c r="C319" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5031,7 +5029,7 @@
         <v>312</v>
       </c>
       <c r="C320" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5042,7 +5040,7 @@
         <v>313</v>
       </c>
       <c r="C321" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5053,7 +5051,7 @@
         <v>314</v>
       </c>
       <c r="C322" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5064,7 +5062,7 @@
         <v>315</v>
       </c>
       <c r="C323" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5075,7 +5073,7 @@
         <v>316</v>
       </c>
       <c r="C324" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5086,7 +5084,7 @@
         <v>317</v>
       </c>
       <c r="C325" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5097,7 +5095,7 @@
         <v>318</v>
       </c>
       <c r="C326" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5108,7 +5106,7 @@
         <v>319</v>
       </c>
       <c r="C327" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5119,7 +5117,7 @@
         <v>320</v>
       </c>
       <c r="C328" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5130,7 +5128,7 @@
         <v>321</v>
       </c>
       <c r="C329" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5141,7 +5139,7 @@
         <v>322</v>
       </c>
       <c r="C330" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5152,7 +5150,7 @@
         <v>323</v>
       </c>
       <c r="C331" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5163,7 +5161,7 @@
         <v>324</v>
       </c>
       <c r="C332" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,7 +5172,7 @@
         <v>325</v>
       </c>
       <c r="C333" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5193,7 +5191,7 @@
         <v>327</v>
       </c>
       <c r="C336" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5204,7 +5202,7 @@
         <v>328</v>
       </c>
       <c r="C337" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5215,7 +5213,7 @@
         <v>329</v>
       </c>
       <c r="C338" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5226,7 +5224,7 @@
         <v>330</v>
       </c>
       <c r="C339" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5237,7 +5235,7 @@
         <v>331</v>
       </c>
       <c r="C340" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,7 +5246,7 @@
         <v>332</v>
       </c>
       <c r="C341" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5259,7 +5257,7 @@
         <v>333</v>
       </c>
       <c r="C342" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5270,7 +5268,7 @@
         <v>334</v>
       </c>
       <c r="C343" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5281,7 +5279,7 @@
         <v>335</v>
       </c>
       <c r="C344" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5292,7 +5290,7 @@
         <v>336</v>
       </c>
       <c r="C345" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5303,7 +5301,7 @@
         <v>337</v>
       </c>
       <c r="C346" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5314,7 +5312,7 @@
         <v>338</v>
       </c>
       <c r="C347" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5325,7 +5323,7 @@
         <v>339</v>
       </c>
       <c r="C348" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5336,7 +5334,7 @@
         <v>340</v>
       </c>
       <c r="C349" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5347,7 +5345,7 @@
         <v>341</v>
       </c>
       <c r="C350" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5358,7 +5356,7 @@
         <v>342</v>
       </c>
       <c r="C351" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5369,7 +5367,7 @@
         <v>343</v>
       </c>
       <c r="C352" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5380,7 +5378,7 @@
         <v>344</v>
       </c>
       <c r="C353" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5399,7 +5397,7 @@
         <v>346</v>
       </c>
       <c r="C356" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5410,7 +5408,7 @@
         <v>347</v>
       </c>
       <c r="C357" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5421,7 +5419,7 @@
         <v>348</v>
       </c>
       <c r="C358" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5432,7 +5430,7 @@
         <v>349</v>
       </c>
       <c r="C359" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5443,7 +5441,7 @@
         <v>350</v>
       </c>
       <c r="C360" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5454,7 +5452,7 @@
         <v>351</v>
       </c>
       <c r="C361" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5465,7 +5463,7 @@
         <v>352</v>
       </c>
       <c r="C362" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5476,7 +5474,7 @@
         <v>353</v>
       </c>
       <c r="C363" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5487,7 +5485,7 @@
         <v>354</v>
       </c>
       <c r="C364" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5498,7 +5496,7 @@
         <v>355</v>
       </c>
       <c r="C365" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5509,7 +5507,7 @@
         <v>356</v>
       </c>
       <c r="C366" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5520,7 +5518,7 @@
         <v>357</v>
       </c>
       <c r="C367" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5531,7 +5529,7 @@
         <v>358</v>
       </c>
       <c r="C368" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5542,7 +5540,7 @@
         <v>359</v>
       </c>
       <c r="C369" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5553,7 +5551,7 @@
         <v>360</v>
       </c>
       <c r="C370" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5564,7 +5562,7 @@
         <v>361</v>
       </c>
       <c r="C371" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5575,7 +5573,7 @@
         <v>362</v>
       </c>
       <c r="C372" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5586,7 +5584,7 @@
         <v>363</v>
       </c>
       <c r="C373" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5597,7 +5595,7 @@
         <v>364</v>
       </c>
       <c r="C374" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5608,7 +5606,7 @@
         <v>365</v>
       </c>
       <c r="C375" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5619,7 +5617,7 @@
         <v>366</v>
       </c>
       <c r="C376" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5630,7 +5628,7 @@
         <v>367</v>
       </c>
       <c r="C377" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5641,7 +5639,7 @@
         <v>368</v>
       </c>
       <c r="C378" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5652,7 +5650,7 @@
         <v>369</v>
       </c>
       <c r="C379" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5663,7 +5661,7 @@
         <v>370</v>
       </c>
       <c r="C380" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5674,7 +5672,7 @@
         <v>371</v>
       </c>
       <c r="C381" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5685,7 +5683,7 @@
         <v>372</v>
       </c>
       <c r="C382" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,7 +5694,7 @@
         <v>373</v>
       </c>
       <c r="C383" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5707,7 +5705,7 @@
         <v>374</v>
       </c>
       <c r="C384" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5718,7 +5716,7 @@
         <v>375</v>
       </c>
       <c r="C385" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5729,7 +5727,7 @@
         <v>376</v>
       </c>
       <c r="C386" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5740,7 +5738,7 @@
         <v>377</v>
       </c>
       <c r="C387" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5751,7 +5749,7 @@
         <v>378</v>
       </c>
       <c r="C388" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5762,7 +5760,7 @@
         <v>379</v>
       </c>
       <c r="C389" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5773,7 +5771,7 @@
         <v>379</v>
       </c>
       <c r="C390" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5784,7 +5782,7 @@
         <v>380</v>
       </c>
       <c r="C391" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5795,7 +5793,7 @@
         <v>381</v>
       </c>
       <c r="C392" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5806,7 +5804,7 @@
         <v>382</v>
       </c>
       <c r="C393" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5817,7 +5815,7 @@
         <v>383</v>
       </c>
       <c r="C394" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5828,7 +5826,7 @@
         <v>384</v>
       </c>
       <c r="C395" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5839,7 +5837,7 @@
         <v>385</v>
       </c>
       <c r="C396" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5850,7 +5848,7 @@
         <v>386</v>
       </c>
       <c r="C397" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5861,7 +5859,7 @@
         <v>387</v>
       </c>
       <c r="C398" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5872,7 +5870,7 @@
         <v>388</v>
       </c>
       <c r="C399" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5891,7 +5889,7 @@
         <v>390</v>
       </c>
       <c r="C402" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5902,7 +5900,7 @@
         <v>391</v>
       </c>
       <c r="C403" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5913,7 +5911,7 @@
         <v>392</v>
       </c>
       <c r="C404" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5924,7 +5922,7 @@
         <v>91</v>
       </c>
       <c r="C405" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5935,7 +5933,7 @@
         <v>393</v>
       </c>
       <c r="C406" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5946,7 +5944,7 @@
         <v>394</v>
       </c>
       <c r="C407" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5965,7 +5963,7 @@
         <v>396</v>
       </c>
       <c r="C410" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5976,7 +5974,7 @@
         <v>397</v>
       </c>
       <c r="C411" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5987,7 +5985,7 @@
         <v>398</v>
       </c>
       <c r="C412" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,7 +5996,7 @@
         <v>399</v>
       </c>
       <c r="C413" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6009,7 +6007,7 @@
         <v>400</v>
       </c>
       <c r="C414" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6020,7 +6018,7 @@
         <v>401</v>
       </c>
       <c r="C415" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6031,7 +6029,7 @@
         <v>402</v>
       </c>
       <c r="C416" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6042,7 +6040,7 @@
         <v>275</v>
       </c>
       <c r="C417" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6053,7 +6051,7 @@
         <v>403</v>
       </c>
       <c r="C418" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6064,7 +6062,7 @@
         <v>404</v>
       </c>
       <c r="C419" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6075,7 +6073,7 @@
         <v>405</v>
       </c>
       <c r="C420" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6086,7 +6084,7 @@
         <v>406</v>
       </c>
       <c r="C421" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6097,7 +6095,7 @@
         <v>407</v>
       </c>
       <c r="C422" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6108,7 +6106,7 @@
         <v>408</v>
       </c>
       <c r="C423" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6119,7 +6117,7 @@
         <v>409</v>
       </c>
       <c r="C424" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6130,7 +6128,7 @@
         <v>410</v>
       </c>
       <c r="C425" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6141,7 +6139,7 @@
         <v>411</v>
       </c>
       <c r="C426" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6152,7 +6150,7 @@
         <v>412</v>
       </c>
       <c r="C427" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6163,7 +6161,7 @@
         <v>413</v>
       </c>
       <c r="C428" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6174,7 +6172,7 @@
         <v>414</v>
       </c>
       <c r="C429" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6185,7 +6183,7 @@
         <v>415</v>
       </c>
       <c r="C430" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6196,7 +6194,7 @@
         <v>416</v>
       </c>
       <c r="C431" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6207,7 +6205,7 @@
         <v>417</v>
       </c>
       <c r="C432" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6218,7 +6216,7 @@
         <v>418</v>
       </c>
       <c r="C433" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6229,7 +6227,7 @@
         <v>419</v>
       </c>
       <c r="C434" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6240,7 +6238,7 @@
         <v>420</v>
       </c>
       <c r="C435" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6251,7 +6249,7 @@
         <v>421</v>
       </c>
       <c r="C436" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6262,7 +6260,7 @@
         <v>422</v>
       </c>
       <c r="C437" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6273,7 +6271,7 @@
         <v>423</v>
       </c>
       <c r="C438" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6284,7 +6282,7 @@
         <v>424</v>
       </c>
       <c r="C439" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6295,7 +6293,7 @@
         <v>425</v>
       </c>
       <c r="C440" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6306,7 +6304,7 @@
         <v>426</v>
       </c>
       <c r="C441" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6317,7 +6315,7 @@
         <v>427</v>
       </c>
       <c r="C442" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6328,7 +6326,7 @@
         <v>428</v>
       </c>
       <c r="C443" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6339,7 +6337,7 @@
         <v>429</v>
       </c>
       <c r="C444" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6350,7 +6348,7 @@
         <v>430</v>
       </c>
       <c r="C445" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6361,7 +6359,7 @@
         <v>431</v>
       </c>
       <c r="C446" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6372,7 +6370,7 @@
         <v>432</v>
       </c>
       <c r="C447" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6383,7 +6381,7 @@
         <v>433</v>
       </c>
       <c r="C448" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6394,7 +6392,7 @@
         <v>434</v>
       </c>
       <c r="C449" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6405,7 +6403,7 @@
         <v>435</v>
       </c>
       <c r="C450" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6416,7 +6414,7 @@
         <v>436</v>
       </c>
       <c r="C451" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6427,7 +6425,7 @@
         <v>437</v>
       </c>
       <c r="C452" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6438,7 +6436,7 @@
         <v>438</v>
       </c>
       <c r="C453" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6449,7 +6447,7 @@
         <v>439</v>
       </c>
       <c r="C454" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6460,7 +6458,7 @@
         <v>440</v>
       </c>
       <c r="C455" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,7 +6469,7 @@
         <v>441</v>
       </c>
       <c r="C456" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6482,7 +6480,7 @@
         <v>442</v>
       </c>
       <c r="C457" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6493,7 +6491,7 @@
         <v>443</v>
       </c>
       <c r="C458" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6504,7 +6502,7 @@
         <v>444</v>
       </c>
       <c r="C459" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6515,7 +6513,7 @@
         <v>445</v>
       </c>
       <c r="C460" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6526,7 +6524,7 @@
         <v>446</v>
       </c>
       <c r="C461" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6537,7 +6535,7 @@
         <v>447</v>
       </c>
       <c r="C462" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6548,7 +6546,7 @@
         <v>448</v>
       </c>
       <c r="C463" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6559,7 +6557,7 @@
         <v>449</v>
       </c>
       <c r="C464" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6570,7 +6568,7 @@
         <v>450</v>
       </c>
       <c r="C465" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6581,7 +6579,7 @@
         <v>451</v>
       </c>
       <c r="C466" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6592,7 +6590,7 @@
         <v>452</v>
       </c>
       <c r="C467" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6603,7 +6601,7 @@
         <v>453</v>
       </c>
       <c r="C468" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6614,7 +6612,7 @@
         <v>454</v>
       </c>
       <c r="C469" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6634,7 +6632,7 @@
         <v>456</v>
       </c>
       <c r="C472" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6645,7 +6643,7 @@
         <v>457</v>
       </c>
       <c r="C473" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6656,7 +6654,7 @@
         <v>458</v>
       </c>
       <c r="C474" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6667,7 +6665,7 @@
         <v>459</v>
       </c>
       <c r="C475" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6678,7 +6676,7 @@
         <v>460</v>
       </c>
       <c r="C476" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6689,7 +6687,7 @@
         <v>461</v>
       </c>
       <c r="C477" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6700,7 +6698,7 @@
         <v>462</v>
       </c>
       <c r="C478" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6711,7 +6709,7 @@
         <v>463</v>
       </c>
       <c r="C479" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6722,7 +6720,7 @@
         <v>464</v>
       </c>
       <c r="C480" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6733,7 +6731,7 @@
         <v>465</v>
       </c>
       <c r="C481" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>